<commit_message>
fix missing message from hidden cells
</commit_message>
<xml_diff>
--- a/excel/TestSuite_KillerCells_Key.xlsx
+++ b/excel/TestSuite_KillerCells_Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F7CB73-0366-4F08-AF16-151013E5D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648E7310-1338-4E66-A51A-65EBBBE414ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="3" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Answer</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Mountain View, CA</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>Cell</t>
   </si>
   <si>
@@ -232,27 +229,15 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Sheetname</t>
-  </si>
-  <si>
     <t>check student's answer for zipcode of Columbus</t>
   </si>
   <si>
     <t>check student's answer for zipcode of Mountain View</t>
   </si>
   <si>
-    <t>Descriptions? (Optional)</t>
-  </si>
-  <si>
-    <t>Hidden? (Optional)</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
-    <t>Feedback (Optional)</t>
-  </si>
-  <si>
     <t>This hidden cell has failed for checking Columbus zipcode</t>
   </si>
   <si>
@@ -262,10 +247,22 @@
     <t>This hidden cell has failed for checking New York zipcode</t>
   </si>
   <si>
-    <t>hk</t>
-  </si>
-  <si>
     <t>hk can be switched to k to test just killer functionality</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -631,9 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F335F84-4731-C64E-A0FE-59327EAC8284}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -642,10 +637,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,7 +712,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -729,67 +724,67 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code update to optimize test mode template
</commit_message>
<xml_diff>
--- a/excel/TestSuite_KillerCells_Key.xlsx
+++ b/excel/TestSuite_KillerCells_Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F7CB73-0366-4F08-AF16-151013E5D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0271AA-5359-48FD-9151-42C5FDF071AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="3" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Answer</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Mountain View, CA</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>Cell</t>
   </si>
   <si>
@@ -232,40 +229,37 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Sheetname</t>
-  </si>
-  <si>
     <t>check student's answer for zipcode of Columbus</t>
   </si>
   <si>
     <t>check student's answer for zipcode of Mountain View</t>
   </si>
   <si>
-    <t>Descriptions? (Optional)</t>
-  </si>
-  <si>
-    <t>Hidden? (Optional)</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Feedback (Optional)</t>
-  </si>
-  <si>
-    <t>This hidden cell has failed for checking Columbus zipcode</t>
-  </si>
-  <si>
-    <t>This hidden cell has failed for checking Mountain View zipcode</t>
-  </si>
-  <si>
-    <t>This hidden cell has failed for checking New York zipcode</t>
-  </si>
-  <si>
     <t>hk</t>
   </si>
   <si>
-    <t>hk can be switched to k to test just killer functionality</t>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>This tab did not pass the pre-requisites. Please contact your instructor.</t>
+  </si>
+  <si>
+    <t>Cell B5 must be correct before this tab can be graded.</t>
   </si>
 </sst>
 </file>
@@ -632,7 +626,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -642,10 +636,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:B6"/>
+  <dimension ref="A3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -674,7 +668,7 @@
     <col min="1" max="1" width="16.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -682,28 +676,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>43215</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>43215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>10001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>94041</v>
+        <v>94045</v>
+      </c>
+      <c r="E6">
+        <v>94043</v>
       </c>
     </row>
   </sheetData>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -727,12 +730,12 @@
     <col min="5" max="5" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
@@ -741,55 +744,49 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>